<commit_message>
Asignación correcta y detecta conflictos
</commit_message>
<xml_diff>
--- a/laboratorios.xlsx
+++ b/laboratorios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t xml:space="preserve">Laboratorio</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">0.513L - Laboratorio MAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arduino</t>
   </si>
 </sst>
 </file>
@@ -197,10 +200,10 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30"/>
@@ -227,7 +230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
@@ -370,6 +373,9 @@
       </c>
       <c r="E9" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>